<commit_message>
orientation email sending bug fix
</commit_message>
<xml_diff>
--- a/scripts/testData.xlsx
+++ b/scripts/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">微信用户</t>
   </si>
@@ -81,45 +81,32 @@
     <t xml:space="preserve">Table</t>
   </si>
   <si>
-    <t xml:space="preserve">liu676785882</t>
-  </si>
-  <si>
-    <t xml:space="preserve">山西</t>
-  </si>
-  <si>
-    <t xml:space="preserve">刘钟楷</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liu676785882@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">计算机科学</t>
-  </si>
-  <si>
-    <t xml:space="preserve">本科</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zkliu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">介休</t>
-  </si>
-  <si>
-    <t xml:space="preserve">刘一手</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jpzrcodek@gmail.com</t>
+    <t xml:space="preserve">hi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hhh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hahk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sjdkf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhfakjf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY\ HH:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,13 +131,6 @@
     <font>
       <sz val="10"/>
       <name val="Noto Sans CJK SC Regular"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -197,20 +177,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,20 +203,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -277,59 +246,26 @@
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="n">
-        <v>43338.375</v>
-      </c>
       <c r="H2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>43338.3784722222</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="liu676785882@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId2" display="jpzrcodek@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Best Singer email sending
</commit_message>
<xml_diff>
--- a/scripts/testData.xlsx
+++ b/scripts/testData.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">刘钟楷</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <r>
       <rPr>
@@ -32,7 +29,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">IT</t>
+      <t xml:space="preserve">10</t>
     </r>
     <r>
       <rPr>
@@ -40,14 +37,29 @@
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">部</t>
+      <t xml:space="preserve">：</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Zkshadow</t>
   </si>
   <si>
     <t xml:space="preserve">liu676785882@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">zkshadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11-3 11:33:19</t>
   </si>
 </sst>
 </file>
@@ -83,6 +95,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -95,7 +108,6 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,7 +152,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,7 +169,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,55 +202,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
-        <v>2</v>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="liu676785882@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId2" display="liu676785882@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="liu676785882@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>